<commit_message>
update column regarding changes
</commit_message>
<xml_diff>
--- a/uploads/SampleFile.xlsx
+++ b/uploads/SampleFile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SFIRSTNAME</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Recommend Loan (Y/N)</t>
+  </si>
+  <si>
+    <t>PMIDDLENAME</t>
   </si>
 </sst>
 </file>
@@ -401,11 +404,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -415,15 +416,16 @@
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,21 +445,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>